<commit_message>
ajouté une class pour le nuage de point, j'y est mis les fonction qui lis le fichier et celle qui dessine les points. la classe point devrait juste contenir les coordonnés des points.
</commit_message>
<xml_diff>
--- a/Coordonnées_points.xlsx
+++ b/Coordonnées_points.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -43,6 +43,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -102,8 +103,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -230,23 +239,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>400</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>